<commit_message>
data cleaning for BC
got data cleaning code adjusted for BC version of survey
</commit_message>
<xml_diff>
--- a/data/BC_Data_100220.xlsx
+++ b/data/BC_Data_100220.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lknelson\Documents\GitHub\climate_perceptions\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B6954BE-E787-410D-B5F7-41B9BD9194CC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40DAC8E6-F703-455D-8654-0C0F0B1E4490}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40740" yWindow="1425" windowWidth="15555" windowHeight="14445" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="A1" sheetId="1" r:id="rId1"/>
@@ -7276,8 +7276,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:JS106"/>
   <sheetViews>
-    <sheetView topLeftCell="BN1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView topLeftCell="ER1" workbookViewId="0">
+      <selection activeCell="DN1" sqref="DN1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.85546875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -87057,8 +87057,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C670"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A80" workbookViewId="0">
-      <selection activeCell="C230" sqref="C230"/>
+    <sheetView tabSelected="1" topLeftCell="A570" workbookViewId="0">
+      <selection activeCell="J570" sqref="J570"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.85546875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
continued adjustments to bc survey
</commit_message>
<xml_diff>
--- a/data/BC_Data_100220.xlsx
+++ b/data/BC_Data_100220.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lknelson\Documents\GitHub\climate_perceptions\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40DAC8E6-F703-455D-8654-0C0F0B1E4490}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5060A5E-4A7A-4CD1-8E58-898E750165A0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -87057,8 +87057,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C670"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A570" workbookViewId="0">
-      <selection activeCell="J570" sqref="J570"/>
+    <sheetView tabSelected="1" topLeftCell="A516" workbookViewId="0">
+      <selection activeCell="H467" sqref="H467"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.85546875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>